<commit_message>
Revised designs to include self diagnostics
</commit_message>
<xml_diff>
--- a/Documentation/whisker_system/whisker_module_BOM.xlsx
+++ b/Documentation/whisker_system/whisker_module_BOM.xlsx
@@ -747,7 +747,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,11 +881,11 @@
         <v>0.2</v>
       </c>
       <c r="J3" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K3" s="1">
         <f>Table3[[#This Row],[Price]]*Table3[[#This Row],[Quantity]]</f>
-        <v>8.6</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1382,11 +1382,11 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6">
         <f>SUM(Table3[Quantity])</f>
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K21" s="7">
         <f>SUM(Table3[Total])</f>
-        <v>44.080000000000005</v>
+        <v>44.280000000000008</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>